<commit_message>
Issue #2797399 by tbradbury, smccabe: Allow human-friendly currency symbols in price
</commit_message>
<xml_diff>
--- a/sample_files/sample.xlsx
+++ b/sample_files/sample.xlsx
@@ -245,8 +245,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -254,6 +255,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -376,7 +378,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -394,6 +396,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -481,17 +487,18 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.7854251012146"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.6518218623482"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.1174089068826"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.5506072874494"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.5222672064777"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.25"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,7 +566,7 @@
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="5" t="n">
         <v>15.99</v>
       </c>
       <c r="G3" s="1" t="n">
@@ -582,7 +589,7 @@
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="5" t="n">
         <v>15.99</v>
       </c>
       <c r="G4" s="1" t="n">
@@ -938,7 +945,7 @@
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -947,6 +954,7 @@
       <c r="D20" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="E20" s="0"/>
       <c r="F20" s="1" t="n">
         <v>20</v>
       </c>
@@ -958,9 +966,11 @@
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="C21" s="0"/>
       <c r="D21" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="E21" s="0"/>
       <c r="F21" s="1" t="n">
         <v>20</v>
       </c>
@@ -978,6 +988,7 @@
       <c r="D22" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="E22" s="0"/>
       <c r="F22" s="1" t="n">
         <v>20</v>
       </c>
@@ -995,6 +1006,8 @@
       <c r="D23" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="E23" s="0"/>
+      <c r="F23" s="0"/>
       <c r="G23" s="1" t="n">
         <v>1</v>
       </c>
@@ -1009,6 +1022,7 @@
       <c r="D24" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="E24" s="0"/>
       <c r="F24" s="1" t="s">
         <v>68</v>
       </c>

</xml_diff>